<commit_message>
adicionando as notas do Fórum
</commit_message>
<xml_diff>
--- a/build/ensino/2022/02/primeiro-semestre-de-2022/mes-4-dia-3-ava-mat236.xlsx
+++ b/build/ensino/2022/02/primeiro-semestre-de-2022/mes-4-dia-3-ava-mat236.xlsx
@@ -1,49 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>matricula</t>
-  </si>
-  <si>
-    <t>nota_view</t>
-  </si>
-  <si>
-    <t>nota_post</t>
-  </si>
-  <si>
-    <t>nota</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -51,356 +28,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -408,251 +48,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -660,63 +58,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -999,38 +345,41 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="10.3" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>matricula</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nota_view</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nota_post</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>nota</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>220215280</v>
       </c>
@@ -1044,7 +393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3">
       <c r="A3">
         <v>218215047</v>
       </c>
@@ -1058,7 +407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4">
       <c r="A4">
         <v>216219962</v>
       </c>
@@ -1072,7 +421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5">
       <c r="A5">
         <v>219116697</v>
       </c>
@@ -1086,7 +435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6">
       <c r="A6">
         <v>220215264</v>
       </c>
@@ -1100,7 +449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7">
       <c r="A7">
         <v>218218130</v>
       </c>
@@ -1114,7 +463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8">
       <c r="A8">
         <v>219217094</v>
       </c>
@@ -1128,7 +477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9">
       <c r="A9">
         <v>217220647</v>
       </c>
@@ -1142,7 +491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10">
       <c r="A10">
         <v>217115466</v>
       </c>
@@ -1156,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11">
       <c r="A11">
         <v>218219337</v>
       </c>
@@ -1170,7 +519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12">
       <c r="A12">
         <v>220119434</v>
       </c>
@@ -1184,7 +533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13">
       <c r="A13">
         <v>220216977</v>
       </c>
@@ -1198,7 +547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14">
       <c r="A14">
         <v>220115582</v>
       </c>
@@ -1212,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15">
       <c r="A15">
         <v>220119361</v>
       </c>
@@ -1226,7 +575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16">
       <c r="A16">
         <v>220115575</v>
       </c>
@@ -1240,7 +589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17">
       <c r="A17">
         <v>218125641</v>
       </c>
@@ -1254,7 +603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18">
       <c r="A18">
         <v>218115560</v>
       </c>
@@ -1268,7 +617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19">
       <c r="A19">
         <v>220116110</v>
       </c>
@@ -1282,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20">
       <c r="A20">
         <v>219120258</v>
       </c>
@@ -1296,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21">
       <c r="A21">
         <v>220216974</v>
       </c>
@@ -1310,7 +659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22">
       <c r="A22">
         <v>220215273</v>
       </c>
@@ -1324,7 +673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23">
       <c r="A23">
         <v>220215263</v>
       </c>
@@ -1338,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24">
       <c r="A24">
         <v>219217085</v>
       </c>
@@ -1352,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25">
       <c r="A25">
         <v>219217088</v>
       </c>
@@ -1366,7 +715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26">
       <c r="A26">
         <v>219216358</v>
       </c>
@@ -1380,7 +729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27">
       <c r="A27">
         <v>217115478</v>
       </c>
@@ -1394,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28">
       <c r="A28">
         <v>220115566</v>
       </c>
@@ -1408,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29">
       <c r="A29">
         <v>219215184</v>
       </c>
@@ -1422,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30">
       <c r="A30">
         <v>219120252</v>
       </c>
@@ -1436,7 +785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31">
       <c r="A31">
         <v>219216330</v>
       </c>
@@ -1450,7 +799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32">
       <c r="A32">
         <v>220216978</v>
       </c>
@@ -1464,7 +813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33">
       <c r="A33">
         <v>220215279</v>
       </c>
@@ -1478,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34">
       <c r="A34">
         <v>219215186</v>
       </c>
@@ -1492,7 +841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35">
       <c r="A35">
         <v>218123228</v>
       </c>
@@ -1506,7 +855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36">
       <c r="A36">
         <v>217216760</v>
       </c>
@@ -1520,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37">
       <c r="A37">
         <v>220215947</v>
       </c>
@@ -1534,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38">
       <c r="A38">
         <v>219215119</v>
       </c>
@@ -1548,7 +897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39">
       <c r="A39">
         <v>220215267</v>
       </c>
@@ -1562,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40">
       <c r="A40">
         <v>220215271</v>
       </c>
@@ -1576,7 +925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41">
       <c r="A41">
         <v>218215098</v>
       </c>
@@ -1590,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42">
       <c r="A42">
         <v>217216747</v>
       </c>
@@ -1604,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43">
       <c r="A43">
         <v>219115746</v>
       </c>
@@ -1618,7 +967,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44">
       <c r="A44">
         <v>220119431</v>
       </c>
@@ -1632,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45">
       <c r="A45">
         <v>220215272</v>
       </c>
@@ -1646,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46">
       <c r="A46">
         <v>220115574</v>
       </c>
@@ -1660,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47">
       <c r="A47">
         <v>219217086</v>
       </c>
@@ -1674,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48">
       <c r="A48">
         <v>219116046</v>
       </c>
@@ -1688,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49">
       <c r="A49">
         <v>217215210</v>
       </c>
@@ -1702,7 +1051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50">
       <c r="A50">
         <v>217120002</v>
       </c>
@@ -1716,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51">
       <c r="A51">
         <v>220215924</v>
       </c>
@@ -1732,6 +1081,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>